<commit_message>
Inference and Conclusion pending
</commit_message>
<xml_diff>
--- a/Code/Product_Sales_Prediction/results_final.xlsx
+++ b/Code/Product_Sales_Prediction/results_final.xlsx
@@ -52,12 +52,12 @@
     <t>Stacking (SGD)</t>
   </si>
   <si>
+    <t>StackingCV</t>
+  </si>
+  <si>
     <t>XGB</t>
   </si>
   <si>
-    <t>StackingCV</t>
-  </si>
-  <si>
     <t>Voting</t>
   </si>
   <si>
@@ -70,16 +70,16 @@
     <t>Decision Tree</t>
   </si>
   <si>
+    <t>SVM (SVC)</t>
+  </si>
+  <si>
     <t>Stacking (Logistic)</t>
   </si>
   <si>
-    <t>SVM (SVC)</t>
+    <t>Vecstack</t>
   </si>
   <si>
     <t>Logistic Regression</t>
-  </si>
-  <si>
-    <t>Vecstack</t>
   </si>
   <si>
     <t>Gaussian Naive-Bayes</t>
@@ -510,19 +510,19 @@
         <v>26</v>
       </c>
       <c r="E2">
-        <v>0.730186999109528</v>
+        <v>0.7279608192341941</v>
       </c>
       <c r="F2">
-        <v>0.7493285586392122</v>
+        <v>0.7448522829006267</v>
       </c>
       <c r="G2">
-        <v>0.7196904557179707</v>
+        <v>0.7184801381692574</v>
       </c>
       <c r="H2">
-        <v>0.8179111294726084</v>
+        <v>0.8129162559779494</v>
       </c>
       <c r="I2">
-        <v>837</v>
+        <v>832</v>
       </c>
       <c r="J2">
         <v>803</v>
@@ -531,12 +531,12 @@
         <v>326</v>
       </c>
       <c r="L2">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="1">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
@@ -548,33 +548,33 @@
         <v>26</v>
       </c>
       <c r="E3">
-        <v>0.7306322350845948</v>
+        <v>0.7337488869100623</v>
       </c>
       <c r="F3">
-        <v>0.747538048343778</v>
+        <v>0.7403760071620412</v>
       </c>
       <c r="G3">
-        <v>0.7210708117443869</v>
+        <v>0.7286343612334801</v>
       </c>
       <c r="H3">
-        <v>0.8175709483757345</v>
+        <v>0.812694226357612</v>
       </c>
       <c r="I3">
-        <v>835</v>
+        <v>827</v>
       </c>
       <c r="J3">
-        <v>806</v>
+        <v>821</v>
       </c>
       <c r="K3">
-        <v>323</v>
+        <v>308</v>
       </c>
       <c r="L3">
-        <v>282</v>
+        <v>290</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="1">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
@@ -586,28 +586,28 @@
         <v>26</v>
       </c>
       <c r="E4">
-        <v>0.7319679430097952</v>
+        <v>0.7284060552092609</v>
       </c>
       <c r="F4">
-        <v>0.7493285586392122</v>
+        <v>0.7600716204118174</v>
       </c>
       <c r="G4">
-        <v>0.7221742881794651</v>
+        <v>0.7128463476070529</v>
       </c>
       <c r="H4">
-        <v>0.8161388573245589</v>
+        <v>0.8112177293823691</v>
       </c>
       <c r="I4">
-        <v>837</v>
+        <v>849</v>
       </c>
       <c r="J4">
-        <v>807</v>
+        <v>787</v>
       </c>
       <c r="K4">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="L4">
-        <v>280</v>
+        <v>268</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -624,28 +624,28 @@
         <v>26</v>
       </c>
       <c r="E5">
-        <v>0.7270703472840605</v>
+        <v>0.7310774710596616</v>
       </c>
       <c r="F5">
-        <v>0.747538048343778</v>
+        <v>0.7287376902417189</v>
       </c>
       <c r="G5">
-        <v>0.7161234991423671</v>
+        <v>0.7300448430493274</v>
       </c>
       <c r="H5">
-        <v>0.8102162172020619</v>
+        <v>0.8066502629068595</v>
       </c>
       <c r="I5">
-        <v>835</v>
+        <v>814</v>
       </c>
       <c r="J5">
-        <v>798</v>
+        <v>828</v>
       </c>
       <c r="K5">
-        <v>331</v>
+        <v>301</v>
       </c>
       <c r="L5">
-        <v>282</v>
+        <v>303</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -662,28 +662,28 @@
         <v>26</v>
       </c>
       <c r="E6">
-        <v>0.7315227070347284</v>
+        <v>0.7337488869100623</v>
       </c>
       <c r="F6">
-        <v>0.7538048343777977</v>
+        <v>0.7394807520143241</v>
       </c>
       <c r="G6">
-        <v>0.7196581196581197</v>
+        <v>0.7290379523389232</v>
       </c>
       <c r="H6">
-        <v>0.8079023513729757</v>
+        <v>0.8044402752215738</v>
       </c>
       <c r="I6">
-        <v>842</v>
+        <v>826</v>
       </c>
       <c r="J6">
-        <v>801</v>
+        <v>822</v>
       </c>
       <c r="K6">
-        <v>328</v>
+        <v>307</v>
       </c>
       <c r="L6">
-        <v>275</v>
+        <v>291</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -700,28 +700,28 @@
         <v>26</v>
       </c>
       <c r="E7">
-        <v>0.7190560997328584</v>
+        <v>0.719946571682992</v>
       </c>
       <c r="F7">
-        <v>0.7430617726051925</v>
+        <v>0.7305282005371531</v>
       </c>
       <c r="G7">
-        <v>0.706984667802385</v>
+        <v>0.7132867132867133</v>
       </c>
       <c r="H7">
-        <v>0.8009096077767461</v>
+        <v>0.7985997067623086</v>
       </c>
       <c r="I7">
-        <v>830</v>
+        <v>816</v>
       </c>
       <c r="J7">
-        <v>785</v>
+        <v>801</v>
       </c>
       <c r="K7">
-        <v>344</v>
+        <v>328</v>
       </c>
       <c r="L7">
-        <v>287</v>
+        <v>301</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -738,180 +738,180 @@
         <v>26</v>
       </c>
       <c r="E8">
-        <v>0.6959038290293855</v>
+        <v>0.695013357079252</v>
       </c>
       <c r="F8">
-        <v>0.7332139659803044</v>
+        <v>0.6741271262309758</v>
       </c>
       <c r="G8">
-        <v>0.6802325581395349</v>
+        <v>0.7011173184357542</v>
       </c>
       <c r="H8">
-        <v>0.7700062564775157</v>
+        <v>0.7649689594661141</v>
       </c>
       <c r="I8">
-        <v>819</v>
+        <v>753</v>
       </c>
       <c r="J8">
-        <v>744</v>
+        <v>808</v>
       </c>
       <c r="K8">
-        <v>385</v>
+        <v>321</v>
       </c>
       <c r="L8">
-        <v>298</v>
+        <v>364</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E9">
-        <v>0.6807658058771149</v>
+        <v>0.678539626001781</v>
       </c>
       <c r="F9">
-        <v>0.666965085049239</v>
+        <v>0.6454789615040286</v>
       </c>
       <c r="G9">
-        <v>0.6834862385321101</v>
+        <v>0.6886341929321872</v>
       </c>
       <c r="H9">
-        <v>0.751243960596086</v>
+        <v>0.7510706981959301</v>
       </c>
       <c r="I9">
-        <v>745</v>
+        <v>721</v>
       </c>
       <c r="J9">
-        <v>784</v>
+        <v>803</v>
       </c>
       <c r="K9">
-        <v>345</v>
+        <v>326</v>
       </c>
       <c r="L9">
-        <v>372</v>
+        <v>396</v>
       </c>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E10">
-        <v>0.684772929652716</v>
+        <v>0.6491540516473731</v>
       </c>
       <c r="F10">
-        <v>0.6777081468218442</v>
+        <v>0.5094001790510295</v>
       </c>
       <c r="G10">
-        <v>0.6850678733031674</v>
+        <v>0.7033374536464772</v>
       </c>
       <c r="H10">
-        <v>0.7505402059959099</v>
+        <v>0.740051288842298</v>
       </c>
       <c r="I10">
-        <v>757</v>
+        <v>569</v>
       </c>
       <c r="J10">
-        <v>781</v>
+        <v>889</v>
       </c>
       <c r="K10">
-        <v>348</v>
+        <v>240</v>
       </c>
       <c r="L10">
-        <v>360</v>
+        <v>548</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="1">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E11">
-        <v>0.6625111308993766</v>
+        <v>0.7252894033837934</v>
       </c>
       <c r="F11">
-        <v>0.6633840644583706</v>
+        <v>0.7600716204118174</v>
       </c>
       <c r="G11">
-        <v>0.659839715048976</v>
+        <v>0.7086811352253757</v>
       </c>
       <c r="H11">
-        <v>0.7165109948275028</v>
+        <v>0.7353561553350941</v>
       </c>
       <c r="I11">
-        <v>741</v>
+        <v>849</v>
       </c>
       <c r="J11">
-        <v>747</v>
+        <v>780</v>
       </c>
       <c r="K11">
-        <v>382</v>
+        <v>349</v>
       </c>
       <c r="L11">
-        <v>376</v>
+        <v>268</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="1">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B12" t="s">
         <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E12">
-        <v>0.7154942119323241</v>
+        <v>0.6665182546749777</v>
       </c>
       <c r="F12">
-        <v>0.7726051924798567</v>
+        <v>0.658012533572068</v>
       </c>
       <c r="G12">
-        <v>0.6915064102564102</v>
+        <v>0.6669691470054446</v>
       </c>
       <c r="H12">
-        <v>0.7157977246721694</v>
+        <v>0.7285434143239238</v>
       </c>
       <c r="I12">
-        <v>863</v>
+        <v>735</v>
       </c>
       <c r="J12">
-        <v>744</v>
+        <v>762</v>
       </c>
       <c r="K12">
-        <v>385</v>
+        <v>367</v>
       </c>
       <c r="L12">
-        <v>254</v>
+        <v>382</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -928,28 +928,28 @@
         <v>27</v>
       </c>
       <c r="E13">
-        <v>0.6549421193232413</v>
+        <v>0.6567230632235085</v>
       </c>
       <c r="F13">
-        <v>0.5926589077887198</v>
+        <v>0.5971351835273053</v>
       </c>
       <c r="G13">
-        <v>0.6741344195519349</v>
+        <v>0.6751012145748988</v>
       </c>
       <c r="H13">
-        <v>0.7081151033270345</v>
+        <v>0.7168908240708655</v>
       </c>
       <c r="I13">
-        <v>662</v>
+        <v>667</v>
       </c>
       <c r="J13">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="K13">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="L13">
-        <v>455</v>
+        <v>450</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -966,25 +966,25 @@
         <v>27</v>
       </c>
       <c r="E14">
-        <v>0.5863757791629564</v>
+        <v>0.5894924309884239</v>
       </c>
       <c r="F14">
         <v>0.3267681289167413</v>
       </c>
       <c r="G14">
-        <v>0.6734317343173432</v>
+        <v>0.6822429906542056</v>
       </c>
       <c r="H14">
-        <v>0.641315113159775</v>
+        <v>0.6517199762428306</v>
       </c>
       <c r="I14">
         <v>365</v>
       </c>
       <c r="J14">
-        <v>952</v>
+        <v>959</v>
       </c>
       <c r="K14">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="L14">
         <v>752</v>

</xml_diff>